<commit_message>
completed 2 easy recursion problems
</commit_message>
<xml_diff>
--- a/Assessment_Practice.xlsx
+++ b/Assessment_Practice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabbiegui/Desktop/Personal_Projects/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3847A5D5-51A9-3744-831B-F207E17FF7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF09328A-01CC-0846-AE77-D799E9B32CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{927CDCF0-531C-DF48-BE59-62CCDF59C2B3}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{927CDCF0-531C-DF48-BE59-62CCDF59C2B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,11 +125,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -179,8 +187,169 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>8038</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>200949</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>8037</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1379DE67-9F94-4622-190E-E361A986BC86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2877595" y="200949"/>
+          <a:ext cx="2998164" cy="739494"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Base</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Case: n=0 or 1, return n</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Recursive Case: return fib(n-1) + fib(n-2)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>8038</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>8038</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>16076</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8957D48-877C-DFF2-B7E2-2B0836BF3FFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2877595" y="667152"/>
+          <a:ext cx="2990127" cy="795759"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Similar to fibonacci</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> number problem. The base case is if n=1,2 then return n. Recursive case is potentially memoization?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -468,7 +637,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -479,7 +648,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,7 +657,7 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -512,42 +681,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C1048576 E2">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C1)))</formula>
     </cfRule>
@@ -565,5 +735,6 @@
     <hyperlink ref="F3" r:id="rId4" xr:uid="{67231088-FDD6-004A-BD62-C38CC76FEF4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>